<commit_message>
Added BOMs for rev2.0
</commit_message>
<xml_diff>
--- a/m50,m40,m60 Pnp/Rev 2.0/BOM-speeduino v0.4.3 compatible PCB for m50nv rev2.0.xlsx
+++ b/m50,m40,m60 Pnp/Rev 2.0/BOM-speeduino v0.4.3 compatible PCB for m50nv rev2.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Documents\GitHub\Speeduino-M5x-PCBs\m50,m40,m60 Pnp\Rev 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE0CF37-0E7D-4310-80D1-6AA55BE750A4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88C8A5E-76C8-422B-98F9-374EB0CBC076}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="1125" windowWidth="23475" windowHeight="12540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Component List" sheetId="1" r:id="rId1"/>
@@ -1113,14 +1113,82 @@
     <t>478-11030-1-ND</t>
   </si>
   <si>
-    <t>Q1,Q2,Q3,Q4,Q6,Q10</t>
-  </si>
-  <si>
-    <t>IC1,IC2,IC3</t>
+    <t>Gate Drivers</t>
+  </si>
+  <si>
+    <t>VNLD5090TR-E</t>
+  </si>
+  <si>
+    <t>497-14323-1-ND</t>
+  </si>
+  <si>
+    <t>511-VNLD5090TR-E</t>
+  </si>
+  <si>
+    <t>U6,U7</t>
+  </si>
+  <si>
+    <t>RES 150 OHM 1W 1% AXIAL</t>
+  </si>
+  <si>
+    <t>Vishay</t>
+  </si>
+  <si>
+    <t>594-5073NW150R0J</t>
+  </si>
+  <si>
+    <t>PR01000101500JR500</t>
+  </si>
+  <si>
+    <t>PPC150W-1CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.50KXBK-ND	</t>
   </si>
   <si>
     <r>
-      <t>R10,R13,R16,R19,R21,R23,R24,R29,R30,</t>
+      <t>C11,C12,C17,C20,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Liberation Sans"/>
+      </rPr>
+      <t>C28</t>
+    </r>
+  </si>
+  <si>
+    <t>R9,R12,R15</t>
+  </si>
+  <si>
+    <r>
+      <t>D9,D10,D11,D18,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Liberation Sans"/>
+      </rPr>
+      <t>D20</t>
+    </r>
+  </si>
+  <si>
+    <t>Q1,Q2,Q3</t>
+  </si>
+  <si>
+    <t>IC1,IC2</t>
+  </si>
+  <si>
+    <t>R25,R27,R31</t>
+  </si>
+  <si>
+    <t>LED1,LED2,LED3,LED5,LED6,LED10</t>
+  </si>
+  <si>
+    <r>
+      <t>R10,R13,R16,R21,R23,R24,R29,</t>
     </r>
     <r>
       <rPr>
@@ -1136,7 +1204,7 @@
         <color rgb="FF000000"/>
         <rFont val="Liberation Sans"/>
       </rPr>
-      <t>,R42,R47,R50,R51,R57,R58,</t>
+      <t>,R50,R51,R57,R58,</t>
     </r>
     <r>
       <rPr>
@@ -1162,88 +1230,12 @@
       </rPr>
       <t>R64</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Liberation Sans"/>
-      </rPr>
-      <t>,R71,R73</t>
-    </r>
-  </si>
-  <si>
-    <t>R11,R14,R17,R20,R35,R36,R37,R38,R43,R48,R49,R52,R55,R56,R70,R75</t>
-  </si>
-  <si>
-    <t>LED1,LED2,LED3,LED4,LED5,LED6,LED7,LED8,LED9,LED10,LED11,LED12</t>
-  </si>
-  <si>
-    <t>R1,R3,R26,R28,R33,R34,R44,R61,R76</t>
-  </si>
-  <si>
-    <t>R25,R27,R31,R32,R45,R74</t>
-  </si>
-  <si>
-    <t>R9,R12,R15,R18,R46,R53</t>
-  </si>
-  <si>
-    <r>
-      <t>D3,D4,D9,D10,D11,D12,D18,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Liberation Sans"/>
-      </rPr>
-      <t>D20</t>
-    </r>
-  </si>
-  <si>
-    <t>Gate Drivers</t>
-  </si>
-  <si>
-    <t>VNLD5090TR-E</t>
-  </si>
-  <si>
-    <t>497-14323-1-ND</t>
-  </si>
-  <si>
-    <t>511-VNLD5090TR-E</t>
-  </si>
-  <si>
-    <t>U6,U7</t>
-  </si>
-  <si>
-    <t>RES 150 OHM 1W 1% AXIAL</t>
-  </si>
-  <si>
-    <t>Vishay</t>
-  </si>
-  <si>
-    <t>594-5073NW150R0J</t>
-  </si>
-  <si>
-    <t>PR01000101500JR500</t>
-  </si>
-  <si>
-    <t>PPC150W-1CT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.50KXBK-ND	</t>
-  </si>
-  <si>
-    <r>
-      <t>C11,C12,C17,C20,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Liberation Sans"/>
-      </rPr>
-      <t>C28</t>
-    </r>
+  </si>
+  <si>
+    <t>R11,R14,R17,R35,R37,R38,R48,R49,R55,R56</t>
+  </si>
+  <si>
+    <t>R1,R3,R26,R28,R33,R61</t>
   </si>
 </sst>
 </file>
@@ -2043,8 +2035,8 @@
   </sheetPr>
   <dimension ref="A1:S65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2135,7 +2127,7 @@
       <c r="N2" s="3"/>
       <c r="O2" s="4"/>
       <c r="P2" s="4" t="str">
-        <f>IF(NOT(I2=""),A2&amp;","&amp;I2,"")</f>
+        <f t="shared" ref="P2:P27" si="0">IF(NOT(I2=""),A2&amp;","&amp;I2,"")</f>
         <v/>
       </c>
       <c r="Q2" t="str">
@@ -2180,28 +2172,28 @@
         <v>1.7</v>
       </c>
       <c r="M3" s="6">
-        <f>K3*A3</f>
+        <f t="shared" ref="M3:M11" si="1">K3*A3</f>
         <v>1.7</v>
       </c>
       <c r="N3" s="6">
-        <f>L3*A3</f>
+        <f t="shared" ref="N3:N11" si="2">L3*A3</f>
         <v>1.7</v>
       </c>
       <c r="O3" s="4"/>
       <c r="P3" s="4" t="str">
-        <f>IF(NOT(I3=""),A3&amp;","&amp;I3,"")</f>
+        <f t="shared" si="0"/>
         <v>1,399-3654-ND</v>
       </c>
       <c r="Q3" t="str">
-        <f>"Capacitor - " &amp;A3&amp;"x "&amp;C3</f>
+        <f t="shared" ref="Q3:Q11" si="3">"Capacitor - " &amp;A3&amp;"x "&amp;C3</f>
         <v>Capacitor - 1x 10uF</v>
       </c>
       <c r="R3" t="str">
-        <f>IF(NOT(J3=""),J3&amp;"|"&amp;A3,"")</f>
+        <f t="shared" ref="R3:R27" si="4">IF(NOT(J3=""),J3&amp;"|"&amp;A3,"")</f>
         <v>80-T356G106K035AT|1</v>
       </c>
       <c r="S3" t="str">
-        <f>H3&amp;" "&amp;A3</f>
+        <f t="shared" ref="S3:S27" si="5">H3&amp;" "&amp;A3</f>
         <v>T356G106K035AT 1</v>
       </c>
     </row>
@@ -2242,28 +2234,28 @@
         <v>0.66</v>
       </c>
       <c r="M4" s="6">
-        <f>K4*A4</f>
+        <f t="shared" si="1"/>
         <v>3.3000000000000003</v>
       </c>
       <c r="N4" s="6">
-        <f>L4*A4</f>
+        <f t="shared" si="2"/>
         <v>3.3000000000000003</v>
       </c>
       <c r="O4" s="4"/>
       <c r="P4" s="4" t="str">
-        <f>IF(NOT(I4=""),A4&amp;","&amp;I4,"")</f>
+        <f t="shared" si="0"/>
         <v>5,BC2678CT-ND</v>
       </c>
       <c r="Q4" t="str">
-        <f>"Capacitor - " &amp;A4&amp;"x "&amp;C4</f>
+        <f t="shared" si="3"/>
         <v>Capacitor - 5x 0.22uF</v>
       </c>
       <c r="R4" t="str">
-        <f>IF(NOT(J4=""),J4&amp;"|"&amp;A4,"")</f>
+        <f t="shared" si="4"/>
         <v>594-K224K20X7RF5UH5|5</v>
       </c>
       <c r="S4" t="str">
-        <f>H4&amp;" "&amp;A4</f>
+        <f t="shared" si="5"/>
         <v>K224K20X7RF5UH5 5</v>
       </c>
     </row>
@@ -2304,28 +2296,28 @@
         <v>0.32</v>
       </c>
       <c r="M5" s="6">
-        <f>K5*A5</f>
+        <f t="shared" si="1"/>
         <v>2.2400000000000002</v>
       </c>
       <c r="N5" s="6">
-        <f>L5*A5</f>
+        <f t="shared" si="2"/>
         <v>2.2400000000000002</v>
       </c>
       <c r="O5" s="4"/>
       <c r="P5" s="4" t="str">
-        <f>IF(NOT(I5=""),A5&amp;","&amp;I5,"")</f>
+        <f t="shared" si="0"/>
         <v>7,399-9879-1-ND</v>
       </c>
       <c r="Q5" t="str">
-        <f>"Capacitor - " &amp;A5&amp;"x "&amp;C5</f>
+        <f t="shared" si="3"/>
         <v>Capacitor - 7x 0.1uF / 100nF</v>
       </c>
       <c r="R5" t="str">
-        <f>IF(NOT(J5=""),J5&amp;"|"&amp;A5,"")</f>
+        <f t="shared" si="4"/>
         <v>80-C322C104M5R-TR|7</v>
       </c>
       <c r="S5" t="str">
-        <f>H5&amp;" "&amp;A5</f>
+        <f t="shared" si="5"/>
         <v>C322C104M5R5TA7301 7</v>
       </c>
     </row>
@@ -2366,34 +2358,34 @@
         <v>1.57</v>
       </c>
       <c r="M6" s="6">
-        <f>K6*A6</f>
+        <f t="shared" si="1"/>
         <v>1.57</v>
       </c>
       <c r="N6" s="6">
-        <f>L6*A6</f>
+        <f t="shared" si="2"/>
         <v>1.57</v>
       </c>
       <c r="O6" s="4"/>
       <c r="P6" s="4" t="str">
-        <f>IF(NOT(I6=""),A6&amp;","&amp;I6,"")</f>
+        <f t="shared" si="0"/>
         <v>1,399-3652-ND</v>
       </c>
       <c r="Q6" t="str">
-        <f>"Capacitor - " &amp;A6&amp;"x "&amp;C6</f>
+        <f t="shared" si="3"/>
         <v>Capacitor - 1x 47uF</v>
       </c>
       <c r="R6" t="str">
-        <f>IF(NOT(J6=""),J6&amp;"|"&amp;A6,"")</f>
+        <f t="shared" si="4"/>
         <v>80-T356F476K6AT|1</v>
       </c>
       <c r="S6" t="str">
-        <f>H6&amp;" "&amp;A6</f>
+        <f t="shared" si="5"/>
         <v>T356F476K006AT 1</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="16.5" thickBot="1">
       <c r="A7" s="17">
-        <f t="shared" ref="A7:A10" si="0">LEN(B7)-LEN(SUBSTITUTE(B7,",",""))+1</f>
+        <f t="shared" ref="A7:A10" si="6">LEN(B7)-LEN(SUBSTITUTE(B7,",",""))+1</f>
         <v>2</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -2428,34 +2420,34 @@
         <v>0.43</v>
       </c>
       <c r="M7" s="6">
-        <f>K7*A7</f>
+        <f t="shared" si="1"/>
         <v>1.24</v>
       </c>
       <c r="N7" s="6">
-        <f>L7*A7</f>
+        <f t="shared" si="2"/>
         <v>0.86</v>
       </c>
       <c r="O7" s="4"/>
       <c r="P7" s="4" t="str">
-        <f>IF(NOT(I7=""),A7&amp;","&amp;I7,"")</f>
+        <f t="shared" si="0"/>
         <v>2,478-5120-ND</v>
       </c>
       <c r="Q7" t="str">
-        <f>"Capacitor - " &amp;A7&amp;"x "&amp;C7</f>
+        <f t="shared" si="3"/>
         <v>Capacitor - 2x 0.33uF</v>
       </c>
       <c r="R7" t="str">
-        <f>IF(NOT(J7=""),J7&amp;"|"&amp;A7,"")</f>
+        <f t="shared" si="4"/>
         <v>581-AR215F334K4R|2</v>
       </c>
       <c r="S7" t="str">
-        <f>H7&amp;" "&amp;A7</f>
+        <f t="shared" si="5"/>
         <v>AR215F334K4R 2</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="16.5" thickBot="1">
       <c r="A8" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -2490,38 +2482,38 @@
         <v>0.24</v>
       </c>
       <c r="M8" s="6">
-        <f>K8*A8</f>
+        <f t="shared" si="1"/>
         <v>0.48</v>
       </c>
       <c r="N8" s="6">
-        <f>L8*A8</f>
+        <f t="shared" si="2"/>
         <v>0.48</v>
       </c>
       <c r="O8" s="4"/>
       <c r="P8" s="4" t="str">
-        <f>IF(NOT(I8=""),A8&amp;","&amp;I8,"")</f>
+        <f t="shared" si="0"/>
         <v>2,399-4206-ND</v>
       </c>
       <c r="Q8" t="str">
-        <f>"Capacitor - " &amp;A8&amp;"x "&amp;C8</f>
+        <f t="shared" si="3"/>
         <v>Capacitor - 2x 0.01uF</v>
       </c>
       <c r="R8" t="str">
-        <f>IF(NOT(J8=""),J8&amp;"|"&amp;A8,"")</f>
+        <f t="shared" si="4"/>
         <v>80-C317C103K5R|2</v>
       </c>
       <c r="S8" t="str">
-        <f>H8&amp;" "&amp;A8</f>
+        <f t="shared" si="5"/>
         <v>C317C103K5R5TA 2</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="16.5" thickBot="1">
       <c r="A9" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>17</v>
@@ -2552,34 +2544,34 @@
         <v>0.66</v>
       </c>
       <c r="M9" s="6">
-        <f>K9*A9</f>
+        <f t="shared" si="1"/>
         <v>3.3000000000000003</v>
       </c>
       <c r="N9" s="6">
-        <f>L9*A9</f>
+        <f t="shared" si="2"/>
         <v>3.3000000000000003</v>
       </c>
       <c r="O9" s="4"/>
       <c r="P9" s="4" t="str">
-        <f>IF(NOT(I9=""),A9&amp;","&amp;I9,"")</f>
+        <f t="shared" si="0"/>
         <v>5,399-4390-ND</v>
       </c>
       <c r="Q9" t="str">
-        <f>"Capacitor - " &amp;A9&amp;"x "&amp;C9</f>
+        <f t="shared" si="3"/>
         <v>Capacitor - 5x 1uF</v>
       </c>
       <c r="R9" t="str">
-        <f>IF(NOT(J9=""),J9&amp;"|"&amp;A9,"")</f>
+        <f t="shared" si="4"/>
         <v>80-C330C105M5U|5</v>
       </c>
       <c r="S9" t="str">
-        <f>H9&amp;" "&amp;A9</f>
+        <f t="shared" si="5"/>
         <v>C330C105M5U5TA 5</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="16.5" thickBot="1">
       <c r="A10" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -2614,28 +2606,28 @@
         <v>0.13</v>
       </c>
       <c r="M10" s="6">
-        <f>K10*A10</f>
+        <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
       <c r="N10" s="6">
-        <f>L10*A10</f>
+        <f t="shared" si="2"/>
         <v>0.13</v>
       </c>
       <c r="O10" s="4"/>
       <c r="P10" s="4" t="str">
-        <f>IF(NOT(I10=""),A10&amp;","&amp;I10,"")</f>
+        <f t="shared" si="0"/>
         <v>1,478-11030-1-ND</v>
       </c>
       <c r="Q10" t="str">
-        <f>"Capacitor - " &amp;A10&amp;"x "&amp;C10</f>
+        <f t="shared" si="3"/>
         <v>Capacitor - 1x 1nF</v>
       </c>
       <c r="R10" t="str">
-        <f>IF(NOT(J10=""),J10&amp;"|"&amp;A10,"")</f>
+        <f t="shared" si="4"/>
         <v>581-SR211C102KARTR1|1</v>
       </c>
       <c r="S10" t="str">
-        <f>H10&amp;" "&amp;A10</f>
+        <f t="shared" si="5"/>
         <v>SR211C102KARTR1 1</v>
       </c>
     </row>
@@ -2676,28 +2668,28 @@
         <v>0.25</v>
       </c>
       <c r="M11" s="6">
-        <f>K11*A11</f>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="N11" s="6">
-        <f>L11*A11</f>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="O11" s="4"/>
       <c r="P11" s="4" t="str">
-        <f>IF(NOT(I11=""),A11&amp;","&amp;I11,"")</f>
+        <f t="shared" si="0"/>
         <v>1,399-4243-ND</v>
       </c>
       <c r="Q11" t="str">
-        <f>"Capacitor - " &amp;A11&amp;"x "&amp;C11</f>
+        <f t="shared" si="3"/>
         <v>Capacitor - 1x 4.7nF</v>
       </c>
       <c r="R11" t="str">
-        <f>IF(NOT(J11=""),J11&amp;"|"&amp;A11,"")</f>
+        <f t="shared" si="4"/>
         <v>80-C317C472K1R|1</v>
       </c>
       <c r="S11" t="str">
-        <f>H11&amp;" "&amp;A11</f>
+        <f t="shared" si="5"/>
         <v>C317C472K1R5TA 1</v>
       </c>
     </row>
@@ -2718,15 +2710,15 @@
       <c r="N12" s="6"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4" t="str">
-        <f>IF(NOT(I12=""),A12&amp;","&amp;I12,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="R12" t="str">
-        <f>IF(NOT(J12=""),J12&amp;"|"&amp;A12,"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="S12" t="str">
-        <f>H12&amp;" "&amp;A12</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -2776,7 +2768,7 @@
       </c>
       <c r="O13" s="4"/>
       <c r="P13" s="4" t="str">
-        <f>IF(NOT(I13=""),A13&amp;","&amp;I13,"")</f>
+        <f t="shared" si="0"/>
         <v>2,1N5919BGOS-ND</v>
       </c>
       <c r="Q13" t="str">
@@ -2784,11 +2776,11 @@
         <v>Diode - 2x 1N5919BG Zener</v>
       </c>
       <c r="R13" t="str">
-        <f>IF(NOT(J13=""),J13&amp;"|"&amp;A13,"")</f>
+        <f t="shared" si="4"/>
         <v>863-1N5919BRLG|2</v>
       </c>
       <c r="S13" t="str">
-        <f>H13&amp;" "&amp;A13</f>
+        <f t="shared" si="5"/>
         <v>1N5919BG 2</v>
       </c>
     </row>
@@ -2838,7 +2830,7 @@
       </c>
       <c r="O14" s="4"/>
       <c r="P14" s="4" t="str">
-        <f>IF(NOT(I14=""),A14&amp;","&amp;I14,"")</f>
+        <f t="shared" si="0"/>
         <v>3,1N5818-TPCT-ND</v>
       </c>
       <c r="Q14" t="str">
@@ -2846,21 +2838,21 @@
         <v>Diode - 3x 1N5818-TP Schottky</v>
       </c>
       <c r="R14" t="str">
-        <f>IF(NOT(J14=""),J14&amp;"|"&amp;A14,"")</f>
+        <f t="shared" si="4"/>
         <v>833-1N5818-TP|3</v>
       </c>
       <c r="S14" t="str">
-        <f>H14&amp;" "&amp;A14</f>
+        <f t="shared" si="5"/>
         <v>1N5818-TP 3</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="26.25" thickBot="1">
+    <row r="15" spans="1:19" ht="16.5" thickBot="1">
       <c r="A15" s="17">
         <f>LEN(B15)-LEN(SUBSTITUTE(B15,",",""))+1</f>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>281</v>
+        <v>294</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>27</v>
@@ -2890,37 +2882,37 @@
       </c>
       <c r="M15" s="6">
         <f>K15*A15</f>
-        <v>5.64</v>
+        <v>2.82</v>
       </c>
       <c r="N15" s="6">
         <f>L15*A15</f>
-        <v>1.2000000000000002</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="O15" s="4"/>
       <c r="P15" s="4" t="str">
-        <f>IF(NOT(I15=""),A15&amp;","&amp;I15,"")</f>
-        <v>12,160-1139-ND</v>
+        <f t="shared" si="0"/>
+        <v>6,160-1139-ND</v>
       </c>
       <c r="Q15" t="str">
         <f>"Diode - " &amp;A15&amp;"x "&amp;C15</f>
-        <v>Diode - 12x LED-Red</v>
+        <v>Diode - 6x LED-Red</v>
       </c>
       <c r="R15" t="str">
-        <f>IF(NOT(J15=""),J15&amp;"|"&amp;A15,"")</f>
-        <v>859-LTL-4221N|12</v>
+        <f t="shared" si="4"/>
+        <v>859-LTL-4221N|6</v>
       </c>
       <c r="S15" t="str">
-        <f>H15&amp;" "&amp;A15</f>
-        <v>LTL-4221N 12</v>
+        <f t="shared" si="5"/>
+        <v>LTL-4221N 6</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="26.25" thickBot="1">
       <c r="A16" s="17">
         <f>LEN(B16)-LEN(SUBSTITUTE(B16,",",""))+1</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>28</v>
@@ -2952,28 +2944,28 @@
       </c>
       <c r="M16" s="6">
         <f>K16*A16</f>
-        <v>0.88</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="N16" s="6">
         <f>L16*A16</f>
-        <v>0.88</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O16" s="4"/>
       <c r="P16" s="4" t="str">
-        <f>IF(NOT(I16=""),A16&amp;","&amp;I16,"")</f>
-        <v>8,1N4004-TPMSCT-ND</v>
+        <f t="shared" si="0"/>
+        <v>5,1N4004-TPMSCT-ND</v>
       </c>
       <c r="Q16" t="str">
         <f>"Diode - " &amp;A16&amp;"x "&amp;C16</f>
-        <v>Diode - 8x 1N4004</v>
+        <v>Diode - 5x 1N4004</v>
       </c>
       <c r="R16" t="str">
-        <f>IF(NOT(J16=""),J16&amp;"|"&amp;A16,"")</f>
-        <v>833-1N4004-TP|8</v>
+        <f t="shared" si="4"/>
+        <v>833-1N4004-TP|5</v>
       </c>
       <c r="S16" t="str">
-        <f>H16&amp;" "&amp;A16</f>
-        <v>1N4004-TP 8</v>
+        <f t="shared" si="5"/>
+        <v>1N4004-TP 5</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="16.5" thickBot="1">
@@ -2993,19 +2985,19 @@
       <c r="N17" s="6"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4" t="str">
-        <f>IF(NOT(I17=""),A17&amp;","&amp;I17,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="Q17" t="str">
-        <f>A17&amp;"x "&amp;C17</f>
+        <f t="shared" ref="Q17:Q29" si="7">A17&amp;"x "&amp;C17</f>
         <v xml:space="preserve">x </v>
       </c>
       <c r="R17" t="str">
-        <f>IF(NOT(J17=""),J17&amp;"|"&amp;A17,"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="S17" t="str">
-        <f>H17&amp;" "&amp;A17</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -3054,19 +3046,19 @@
       </c>
       <c r="O18" s="4"/>
       <c r="P18" s="4" t="str">
-        <f>IF(NOT(I18=""),A18&amp;","&amp;I18,"")</f>
+        <f t="shared" si="0"/>
         <v>1,P7307-ND</v>
       </c>
       <c r="Q18" t="str">
-        <f>A18&amp;"x "&amp;C18</f>
+        <f t="shared" si="7"/>
         <v>1x Surge Protection</v>
       </c>
       <c r="R18" t="str">
-        <f>IF(NOT(J18=""),J18&amp;"|"&amp;A18,"")</f>
+        <f t="shared" si="4"/>
         <v>667-ERZ-V14D220|1</v>
       </c>
       <c r="S18" t="str">
-        <f>H18&amp;" "&amp;A18</f>
+        <f t="shared" si="5"/>
         <v>ERZ-V14D220 1</v>
       </c>
     </row>
@@ -3087,19 +3079,19 @@
       <c r="N19" s="6"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4" t="str">
-        <f>IF(NOT(I19=""),A19&amp;","&amp;I19,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="Q19" t="str">
-        <f>A19&amp;"x "&amp;C19</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">x </v>
       </c>
       <c r="R19" t="str">
-        <f>IF(NOT(J19=""),J19&amp;"|"&amp;A19,"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="S19" t="str">
-        <f>H19&amp;" "&amp;A19</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -3148,19 +3140,19 @@
         <v>150</v>
       </c>
       <c r="P20" s="4" t="str">
-        <f>IF(NOT(I20=""),A20&amp;","&amp;I20,"")</f>
+        <f t="shared" si="0"/>
         <v>4,S1012EC-40-ND</v>
       </c>
       <c r="Q20" t="str">
-        <f>A20&amp;"x "&amp;C20</f>
+        <f t="shared" si="7"/>
         <v>4x 40 POS 0.100 Pin Header</v>
       </c>
       <c r="R20" t="str">
-        <f>IF(NOT(J20=""),J20&amp;"|"&amp;A20,"")</f>
+        <f t="shared" si="4"/>
         <v>571-41037410|4</v>
       </c>
       <c r="S20" t="str">
-        <f>H20&amp;" "&amp;A20</f>
+        <f t="shared" si="5"/>
         <v>PREC040SAAN-RC.. 4</v>
       </c>
     </row>
@@ -3207,19 +3199,19 @@
       </c>
       <c r="O21" s="4"/>
       <c r="P21" s="4" t="str">
-        <f>IF(NOT(I21=""),A21&amp;","&amp;I21,"")</f>
+        <f t="shared" si="0"/>
         <v>1,WM1353-ND</v>
       </c>
       <c r="Q21" t="str">
-        <f>A21&amp;"x "&amp;C21</f>
+        <f t="shared" si="7"/>
         <v>1x 6 POS Header</v>
       </c>
       <c r="R21" t="str">
-        <f>IF(NOT(J21=""),J21&amp;"|"&amp;A21,"")</f>
+        <f t="shared" si="4"/>
         <v>538-39-30-1060|1</v>
       </c>
       <c r="S21" t="str">
-        <f>H21&amp;" "&amp;A21</f>
+        <f t="shared" si="5"/>
         <v>39-30-1060 1</v>
       </c>
     </row>
@@ -3266,19 +3258,19 @@
       </c>
       <c r="O22" s="4"/>
       <c r="P22" s="4" t="str">
-        <f>IF(NOT(I22=""),A22&amp;","&amp;I22,"")</f>
+        <f t="shared" si="0"/>
         <v>1,WM1353-ND</v>
       </c>
       <c r="Q22" t="str">
-        <f>A22&amp;"x "&amp;C22</f>
+        <f t="shared" si="7"/>
         <v>1x 6 POS Header</v>
       </c>
       <c r="R22" t="str">
-        <f>IF(NOT(J22=""),J22&amp;"|"&amp;A22,"")</f>
+        <f t="shared" si="4"/>
         <v>538-39-30-1060|1</v>
       </c>
       <c r="S22" t="str">
-        <f>H22&amp;" "&amp;A22</f>
+        <f t="shared" si="5"/>
         <v>39-30-1060 1</v>
       </c>
     </row>
@@ -3325,19 +3317,19 @@
       </c>
       <c r="O23" s="4"/>
       <c r="P23" s="4" t="str">
-        <f>IF(NOT(I23=""),A23&amp;","&amp;I23,"")</f>
+        <f t="shared" si="0"/>
         <v>1,SAM1213-04-ND</v>
       </c>
       <c r="Q23" t="str">
-        <f>A23&amp;"x "&amp;C23</f>
+        <f t="shared" si="7"/>
         <v>1x 4 POS Header</v>
       </c>
       <c r="R23" t="str">
-        <f>IF(NOT(J23=""),J23&amp;"|"&amp;A23,"")</f>
+        <f t="shared" si="4"/>
         <v>200-SSW10401TS|1</v>
       </c>
       <c r="S23" t="str">
-        <f>H23&amp;" "&amp;A23</f>
+        <f t="shared" si="5"/>
         <v>SSW-104-01-T-S 1</v>
       </c>
     </row>
@@ -3384,19 +3376,19 @@
       </c>
       <c r="O24" s="4"/>
       <c r="P24" s="4" t="str">
-        <f>IF(NOT(I24=""),A24&amp;","&amp;I24,"")</f>
+        <f t="shared" si="0"/>
         <v>1,SAM1213-02-ND</v>
       </c>
       <c r="Q24" t="str">
-        <f>A24&amp;"x "&amp;C24</f>
+        <f t="shared" si="7"/>
         <v>1x 2 POS Header</v>
       </c>
       <c r="R24" t="str">
-        <f>IF(NOT(J24=""),J24&amp;"|"&amp;A24,"")</f>
+        <f t="shared" si="4"/>
         <v>200-SSW10201TS|1</v>
       </c>
       <c r="S24" t="str">
-        <f>H24&amp;" "&amp;A24</f>
+        <f t="shared" si="5"/>
         <v>SSW-102-01-T-S 1</v>
       </c>
     </row>
@@ -3417,29 +3409,29 @@
       <c r="N25" s="6"/>
       <c r="O25" s="4"/>
       <c r="P25" s="4" t="str">
-        <f>IF(NOT(I25=""),A25&amp;","&amp;I25,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="Q25" t="str">
-        <f>A25&amp;"x "&amp;C25</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">x </v>
       </c>
       <c r="R25" t="str">
-        <f>IF(NOT(J25=""),J25&amp;"|"&amp;A25,"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="S25" t="str">
-        <f>H25&amp;" "&amp;A25</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="26" spans="1:19" ht="26.25" thickBot="1">
       <c r="A26" s="17">
         <f>LEN(B26)-LEN(SUBSTITUTE(B26,",",""))+1</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>89</v>
@@ -3471,28 +3463,28 @@
       </c>
       <c r="M26" s="6">
         <f>K26*A26</f>
-        <v>9.06</v>
+        <v>4.53</v>
       </c>
       <c r="N26" s="6">
         <f>L26*A26</f>
-        <v>9.06</v>
+        <v>4.53</v>
       </c>
       <c r="O26" s="4"/>
       <c r="P26" s="4" t="str">
-        <f>IF(NOT(I26=""),A26&amp;","&amp;I26,"")</f>
-        <v>6,497-5981-5-ND</v>
+        <f t="shared" si="0"/>
+        <v>3,497-5981-5-ND</v>
       </c>
       <c r="Q26" t="str">
-        <f>A26&amp;"x "&amp;C26</f>
-        <v>6x 62A MOSFET N-CH</v>
+        <f t="shared" si="7"/>
+        <v>3x 62A MOSFET N-CH</v>
       </c>
       <c r="R26" t="str">
-        <f>IF(NOT(J26=""),J26&amp;"|"&amp;A26,"")</f>
-        <v>511-STP62NS04Z|6</v>
+        <f t="shared" si="4"/>
+        <v>511-STP62NS04Z|3</v>
       </c>
       <c r="S26" t="str">
-        <f>H26&amp;" "&amp;A26</f>
-        <v>STP75NS04Z 6</v>
+        <f t="shared" si="5"/>
+        <v>STP75NS04Z 3</v>
       </c>
     </row>
     <row r="27" spans="1:19" ht="26.25" thickBot="1">
@@ -3541,20 +3533,20 @@
       </c>
       <c r="O27" s="4"/>
       <c r="P27" s="4" t="str">
-        <f>IF(NOT(I27=""),A27&amp;","&amp;I27,"")</f>
+        <f t="shared" si="0"/>
         <v>6,ISL9V5036P3-F085-ND</v>
       </c>
       <c r="Q27" t="str">
-        <f>A27&amp;"x "&amp;C27</f>
+        <f t="shared" si="7"/>
         <v>6x Ignition IGBT</v>
       </c>
       <c r="R27" t="str">
-        <f>IF(NOT(J27=""),J27&amp;"|"&amp;A27,"")</f>
+        <f t="shared" si="4"/>
         <v>512-ISL9V5036P3-F085
 |6</v>
       </c>
       <c r="S27" t="str">
-        <f>H27&amp;" "&amp;A27</f>
+        <f t="shared" si="5"/>
         <v>ISL9V5036P3-F085 6</v>
       </c>
     </row>
@@ -3608,7 +3600,7 @@
         <v>1,PN2222AFS-ND</v>
       </c>
       <c r="Q28" t="str">
-        <f>A28&amp;"x "&amp;C28</f>
+        <f t="shared" si="7"/>
         <v>1x PNP transistor</v>
       </c>
       <c r="R28" t="str">
@@ -3670,7 +3662,7 @@
         <v>1,PN2907ABUFS-ND</v>
       </c>
       <c r="Q29" t="str">
-        <f>A29&amp;"x "&amp;C29</f>
+        <f t="shared" si="7"/>
         <v>1x NPN transistor</v>
       </c>
       <c r="R29" t="str">
@@ -3788,13 +3780,13 @@
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
     </row>
-    <row r="33" spans="1:19" ht="26.25" thickBot="1">
+    <row r="33" spans="1:19" ht="16.5" thickBot="1">
       <c r="A33" s="17">
         <f>LEN(B33)-LEN(SUBSTITUTE(B33,",",""))+1</f>
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>279</v>
+        <v>295</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>43</v>
@@ -3823,38 +3815,38 @@
         <v>0.11</v>
       </c>
       <c r="M33" s="6">
-        <f>K33*A33</f>
-        <v>1.26</v>
+        <f t="shared" ref="M33:M40" si="8">K33*A33</f>
+        <v>0.89999999999999991</v>
       </c>
       <c r="N33" s="6">
-        <f>L33*A33</f>
-        <v>2.31</v>
+        <f t="shared" ref="N33:N40" si="9">L33*A33</f>
+        <v>1.65</v>
       </c>
       <c r="O33" s="4"/>
       <c r="P33" s="4" t="str">
-        <f>IF(NOT(I33=""),A33&amp;","&amp;I33,"")</f>
-        <v>21,1.00KXBK-ND</v>
+        <f t="shared" ref="P33:P42" si="10">IF(NOT(I33=""),A33&amp;","&amp;I33,"")</f>
+        <v>15,1.00KXBK-ND</v>
       </c>
       <c r="Q33" t="str">
-        <f>"Resistor - " &amp; A33&amp;"x "&amp;C33</f>
-        <v>Resistor - 21x 1k</v>
+        <f t="shared" ref="Q33:Q40" si="11">"Resistor - " &amp; A33&amp;"x "&amp;C33</f>
+        <v>Resistor - 15x 1k</v>
       </c>
       <c r="R33" t="str">
-        <f>IF(NOT(J33=""),J33&amp;"|"&amp;A33,"")</f>
-        <v>603-MFR-25FBF52-1K|21</v>
+        <f t="shared" ref="R33:R42" si="12">IF(NOT(J33=""),J33&amp;"|"&amp;A33,"")</f>
+        <v>603-MFR-25FBF52-1K|15</v>
       </c>
       <c r="S33" t="str">
-        <f>H33&amp;" "&amp;A33</f>
-        <v>MFR-25FBF52-1K 21</v>
+        <f t="shared" ref="S33:S42" si="13">H33&amp;" "&amp;A33</f>
+        <v>MFR-25FBF52-1K 15</v>
       </c>
     </row>
     <row r="34" spans="1:19" ht="16.5" thickBot="1">
       <c r="A34" s="17">
         <f>LEN(B34)-LEN(SUBSTITUTE(B34,",",""))+1</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="C34" s="12">
         <v>680</v>
@@ -3883,31 +3875,31 @@
         <v>0.15</v>
       </c>
       <c r="M34" s="6">
-        <f>K34*A34</f>
-        <v>1.32</v>
+        <f t="shared" si="8"/>
+        <v>0.66</v>
       </c>
       <c r="N34" s="6">
-        <f>L34*A34</f>
-        <v>0.89999999999999991</v>
+        <f t="shared" si="9"/>
+        <v>0.44999999999999996</v>
       </c>
       <c r="O34" s="11" t="s">
         <v>79</v>
       </c>
       <c r="P34" s="4" t="str">
-        <f>IF(NOT(I34=""),A34&amp;","&amp;I34,"")</f>
-        <v>6,A105963CT-ND</v>
+        <f t="shared" si="10"/>
+        <v>3,A105963CT-ND</v>
       </c>
       <c r="Q34" t="str">
-        <f>"Resistor - " &amp; A34&amp;"x "&amp;C34</f>
-        <v>Resistor - 6x 680</v>
+        <f t="shared" si="11"/>
+        <v>Resistor - 3x 680</v>
       </c>
       <c r="R34" t="str">
-        <f>IF(NOT(J34=""),J34&amp;"|"&amp;A34,"")</f>
-        <v>279-LR1F680R|6</v>
+        <f t="shared" si="12"/>
+        <v>279-LR1F680R|3</v>
       </c>
       <c r="S34" t="str">
-        <f>H34&amp;" "&amp;A34</f>
-        <v>1622545-1 6</v>
+        <f t="shared" si="13"/>
+        <v>1622545-1 3</v>
       </c>
     </row>
     <row r="35" spans="1:19" ht="26.25" thickBot="1">
@@ -3945,38 +3937,38 @@
         <v>0.15</v>
       </c>
       <c r="M35" s="6">
-        <f>K35*A35</f>
+        <f t="shared" si="8"/>
         <v>0.66</v>
       </c>
       <c r="N35" s="6">
-        <f>L35*A35</f>
+        <f t="shared" si="9"/>
         <v>0.89999999999999991</v>
       </c>
       <c r="O35" s="4"/>
       <c r="P35" s="4" t="str">
-        <f>IF(NOT(I35=""),A35&amp;","&amp;I35,"")</f>
+        <f t="shared" si="10"/>
         <v>6,RNF14FTD470RCT-ND</v>
       </c>
       <c r="Q35" t="str">
-        <f>"Resistor - " &amp; A35&amp;"x "&amp;C35</f>
+        <f t="shared" si="11"/>
         <v>Resistor - 6x 470</v>
       </c>
       <c r="R35" t="str">
-        <f>IF(NOT(J35=""),J35&amp;"|"&amp;A35,"")</f>
+        <f t="shared" si="12"/>
         <v>279-LR1F470R|6</v>
       </c>
       <c r="S35" t="str">
-        <f>H35&amp;" "&amp;A35</f>
+        <f t="shared" si="13"/>
         <v>RNF14FTD470R 6</v>
       </c>
     </row>
     <row r="36" spans="1:19" ht="26.25" thickBot="1">
       <c r="A36" s="17">
-        <f t="shared" ref="A36:A37" si="1">LEN(B36)-LEN(SUBSTITUTE(B36,",",""))+1</f>
-        <v>9</v>
+        <f t="shared" ref="A36:A37" si="14">LEN(B36)-LEN(SUBSTITUTE(B36,",",""))+1</f>
+        <v>6</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>282</v>
+        <v>297</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>164</v>
@@ -4007,34 +3999,34 @@
         <v>0.16</v>
       </c>
       <c r="M36" s="6">
-        <f>K36*A36</f>
-        <v>1.2600000000000002</v>
+        <f t="shared" si="8"/>
+        <v>0.84000000000000008</v>
       </c>
       <c r="N36" s="6">
-        <f>L36*A36</f>
-        <v>1.44</v>
+        <f t="shared" si="9"/>
+        <v>0.96</v>
       </c>
       <c r="O36" s="4"/>
       <c r="P36" s="4" t="str">
-        <f>IF(NOT(I36=""),A36&amp;","&amp;I36,"")</f>
-        <v>9,2.49KXBK-ND</v>
+        <f t="shared" si="10"/>
+        <v>6,2.49KXBK-ND</v>
       </c>
       <c r="Q36" t="str">
-        <f>"Resistor - " &amp; A36&amp;"x "&amp;C36</f>
-        <v>Resistor - 9x 1% 2.49k</v>
+        <f t="shared" si="11"/>
+        <v>Resistor - 6x 1% 2.49k</v>
       </c>
       <c r="R36" t="str">
-        <f>IF(NOT(J36=""),J36&amp;"|"&amp;A36,"")</f>
-        <v>603-MFR-25FBF52-2K49|9</v>
+        <f t="shared" si="12"/>
+        <v>603-MFR-25FBF52-2K49|6</v>
       </c>
       <c r="S36" t="str">
-        <f>H36&amp;" "&amp;A36</f>
-        <v>MFR-25FBF52-2K49 9</v>
+        <f t="shared" si="13"/>
+        <v>MFR-25FBF52-2K49 6</v>
       </c>
     </row>
     <row r="37" spans="1:19" ht="16.5" thickBot="1">
       <c r="A37" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="B37" s="4" t="s">
@@ -4067,40 +4059,40 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="M37" s="6">
-        <f>K37*A37</f>
+        <f t="shared" si="8"/>
         <v>1.3800000000000001</v>
       </c>
       <c r="N37" s="6">
-        <f>L37*A37</f>
+        <f t="shared" si="9"/>
         <v>3.3000000000000003</v>
       </c>
       <c r="O37" s="4" t="s">
         <v>78</v>
       </c>
       <c r="P37" s="4" t="str">
-        <f>IF(NOT(I37=""),A37&amp;","&amp;I37,"")</f>
+        <f t="shared" si="10"/>
         <v>3,3.9KADCT-ND</v>
       </c>
       <c r="Q37" t="str">
-        <f>"Resistor - " &amp; A37&amp;"x "&amp;C37</f>
+        <f t="shared" si="11"/>
         <v>Resistor - 3x 0.1% 3.9k</v>
       </c>
       <c r="R37" t="str">
-        <f>IF(NOT(J37=""),J37&amp;"|"&amp;A37,"")</f>
+        <f t="shared" si="12"/>
         <v>279-H83K9BDA|3</v>
       </c>
       <c r="S37" t="str">
-        <f>H37&amp;" "&amp;A37</f>
+        <f t="shared" si="13"/>
         <v>MFP-25BRD52-3K9 3</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="26.25" thickBot="1">
+    <row r="38" spans="1:19" ht="16.5" thickBot="1">
       <c r="A38" s="17">
-        <f t="shared" ref="A38" si="2">LEN(B38)-LEN(SUBSTITUTE(B38,",",""))+1</f>
-        <v>16</v>
+        <f t="shared" ref="A38" si="15">LEN(B38)-LEN(SUBSTITUTE(B38,",",""))+1</f>
+        <v>10</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>280</v>
+        <v>296</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>54</v>
@@ -4129,58 +4121,58 @@
         <v>0.1</v>
       </c>
       <c r="M38" s="6">
-        <f>K38*A38</f>
-        <v>1.6</v>
+        <f t="shared" si="8"/>
+        <v>1</v>
       </c>
       <c r="N38" s="6">
-        <f>L38*A38</f>
-        <v>1.6</v>
+        <f t="shared" si="9"/>
+        <v>1</v>
       </c>
       <c r="O38" s="4"/>
       <c r="P38" s="4" t="str">
-        <f>IF(NOT(I38=""),A38&amp;","&amp;I38,"")</f>
-        <v>16,100KXBK-ND</v>
+        <f t="shared" si="10"/>
+        <v>10,100KXBK-ND</v>
       </c>
       <c r="Q38" t="str">
-        <f>"Resistor - " &amp; A38&amp;"x "&amp;C38</f>
-        <v>Resistor - 16x 100k</v>
+        <f t="shared" si="11"/>
+        <v>Resistor - 10x 100k</v>
       </c>
       <c r="R38" t="str">
-        <f>IF(NOT(J38=""),J38&amp;"|"&amp;A38,"")</f>
-        <v>603-FMF-25FTF52100K|16</v>
+        <f t="shared" si="12"/>
+        <v>603-FMF-25FTF52100K|10</v>
       </c>
       <c r="S38" t="str">
-        <f>H38&amp;" "&amp;A38</f>
-        <v>MFR-25FBF52-100K 16</v>
+        <f t="shared" si="13"/>
+        <v>MFR-25FBF52-100K 10</v>
       </c>
     </row>
     <row r="39" spans="1:19" ht="16.5" thickBot="1">
       <c r="A39" s="17">
         <f>LEN(B39)-LEN(SUBSTITUTE(B39,",",""))+1</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="C39" s="3">
         <v>150</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="K39" s="5">
         <v>0.27</v>
@@ -4189,29 +4181,29 @@
         <v>0.23</v>
       </c>
       <c r="M39" s="6">
-        <f>K39*A39</f>
-        <v>1.62</v>
+        <f t="shared" si="8"/>
+        <v>0.81</v>
       </c>
       <c r="N39" s="6">
-        <f>L39*A39</f>
-        <v>1.3800000000000001</v>
+        <f t="shared" si="9"/>
+        <v>0.69000000000000006</v>
       </c>
       <c r="O39" s="4"/>
       <c r="P39" s="4" t="str">
-        <f>IF(NOT(I39=""),A39&amp;","&amp;I39,"")</f>
-        <v>6,PPC150W-1CT-ND</v>
+        <f t="shared" si="10"/>
+        <v>3,PPC150W-1CT-ND</v>
       </c>
       <c r="Q39" t="str">
-        <f>"Resistor - " &amp; A39&amp;"x "&amp;C39</f>
-        <v>Resistor - 6x 150</v>
+        <f t="shared" si="11"/>
+        <v>Resistor - 3x 150</v>
       </c>
       <c r="R39" t="str">
-        <f>IF(NOT(J39=""),J39&amp;"|"&amp;A39,"")</f>
-        <v>594-5073NW150R0J|6</v>
+        <f t="shared" si="12"/>
+        <v>594-5073NW150R0J|3</v>
       </c>
       <c r="S39" t="str">
-        <f>H39&amp;" "&amp;A39</f>
-        <v>PR01000101500JR500 6</v>
+        <f t="shared" si="13"/>
+        <v>PR01000101500JR500 3</v>
       </c>
     </row>
     <row r="40" spans="1:19" ht="26.25" thickBot="1">
@@ -4237,7 +4229,7 @@
         <v>182</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="J40" s="2" t="s">
         <v>183</v>
@@ -4247,29 +4239,29 @@
         <v>0.1</v>
       </c>
       <c r="M40" s="6">
-        <f>K40*A40</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="N40" s="6">
-        <f>L40*A40</f>
+        <f t="shared" si="9"/>
         <v>0.2</v>
       </c>
       <c r="O40" s="4"/>
       <c r="P40" s="4" t="str">
-        <f>IF(NOT(I40=""),A40&amp;","&amp;I40,"")</f>
+        <f t="shared" si="10"/>
         <v xml:space="preserve">2,7.50KXBK-ND	</v>
       </c>
       <c r="Q40" t="str">
-        <f>"Resistor - " &amp; A40&amp;"x "&amp;C40</f>
+        <f t="shared" si="11"/>
         <v>Resistor - 2x 7.5k</v>
       </c>
       <c r="R40" t="str">
-        <f>IF(NOT(J40=""),J40&amp;"|"&amp;A40,"")</f>
+        <f t="shared" si="12"/>
         <v>603-MFR-25FBF52-7K5
 |2</v>
       </c>
       <c r="S40" t="str">
-        <f>H40&amp;" "&amp;A40</f>
+        <f t="shared" si="13"/>
         <v>MFR-25FBF52-7K5 2</v>
       </c>
     </row>
@@ -4290,21 +4282,21 @@
       <c r="N41" s="6"/>
       <c r="O41" s="4"/>
       <c r="P41" s="4" t="str">
-        <f>IF(NOT(I41=""),A41&amp;","&amp;I41,"")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="R41" t="str">
-        <f>IF(NOT(J41=""),J41&amp;"|"&amp;A41,"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="S41" t="str">
-        <f>H41&amp;" "&amp;A41</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="42" spans="1:19" ht="26.25" thickBot="1">
       <c r="A42" s="17">
-        <f>LEN(B42)-LEN(SUBSTITUTE(B42,",",""))+1</f>
+        <f t="shared" ref="A42:A48" si="16">LEN(B42)-LEN(SUBSTITUTE(B42,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B42" s="4" t="s">
@@ -4348,7 +4340,7 @@
       </c>
       <c r="O42" s="4"/>
       <c r="P42" s="4" t="str">
-        <f>IF(NOT(I42=""),A42&amp;","&amp;I42,"")</f>
+        <f t="shared" si="10"/>
         <v>1,LM2940T-5.0/NOPB</v>
       </c>
       <c r="Q42" t="str">
@@ -4356,17 +4348,17 @@
         <v>1x LM2940T-5.0/NOPB</v>
       </c>
       <c r="R42" t="str">
-        <f>IF(NOT(J42=""),J42&amp;"|"&amp;A42,"")</f>
+        <f t="shared" si="12"/>
         <v>926-LM2940T-5.0/NOPB|1</v>
       </c>
       <c r="S42" t="str">
-        <f>H42&amp;" "&amp;A42</f>
+        <f t="shared" si="13"/>
         <v>LM2940T-5.0/NOPB 1</v>
       </c>
     </row>
     <row r="43" spans="1:19" ht="16.5" thickBot="1">
       <c r="A43" s="17">
-        <f>LEN(B43)-LEN(SUBSTITUTE(B43,",",""))+1</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="B43" s="4" t="s">
@@ -4422,7 +4414,7 @@
     </row>
     <row r="44" spans="1:19" ht="26.25" thickBot="1">
       <c r="A44" s="17">
-        <f>LEN(B44)-LEN(SUBSTITUTE(B44,",",""))+1</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="B44" s="21" t="s">
@@ -4466,7 +4458,7 @@
       </c>
       <c r="O44" s="4"/>
       <c r="P44" s="4" t="str">
-        <f>IF(NOT(I44=""),A44&amp;","&amp;I44,"")</f>
+        <f t="shared" ref="P44:P50" si="17">IF(NOT(I44=""),A44&amp;","&amp;I44,"")</f>
         <v>1,MPXH6115A6U-ND</v>
       </c>
       <c r="Q44" t="str">
@@ -4474,7 +4466,7 @@
         <v>1x Baro sensor</v>
       </c>
       <c r="R44" t="str">
-        <f>IF(NOT(J44=""),J44&amp;"|"&amp;A44,"")</f>
+        <f t="shared" ref="R44:R50" si="18">IF(NOT(J44=""),J44&amp;"|"&amp;A44,"")</f>
         <v>841-MPXH6115A6U|1</v>
       </c>
       <c r="S44" t="str">
@@ -4484,7 +4476,7 @@
     </row>
     <row r="45" spans="1:19" ht="26.25" thickBot="1">
       <c r="A45" s="17">
-        <f>LEN(B45)-LEN(SUBSTITUTE(B45,",",""))+1</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="B45" s="4" t="s">
@@ -4528,7 +4520,7 @@
       </c>
       <c r="O45" s="4"/>
       <c r="P45" s="4" t="str">
-        <f>IF(NOT(I45=""),A45&amp;","&amp;I45,"")</f>
+        <f t="shared" si="17"/>
         <v>1,MPX4250AP-ND</v>
       </c>
       <c r="Q45" t="str">
@@ -4536,7 +4528,7 @@
         <v>1x 2.5-Bar MAP sensor</v>
       </c>
       <c r="R45" t="str">
-        <f>IF(NOT(J45=""),J45&amp;"|"&amp;A45,"")</f>
+        <f t="shared" si="18"/>
         <v>841-MPX4250AP|1</v>
       </c>
       <c r="S45" t="str">
@@ -4546,11 +4538,11 @@
     </row>
     <row r="46" spans="1:19" ht="26.25" thickBot="1">
       <c r="A46" s="17">
-        <f>LEN(B46)-LEN(SUBSTITUTE(B46,",",""))+1</f>
-        <v>3</v>
+        <f t="shared" si="16"/>
+        <v>2</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>278</v>
+        <v>292</v>
       </c>
       <c r="C46" s="12" t="s">
         <v>94</v>
@@ -4582,33 +4574,33 @@
       </c>
       <c r="M46" s="6">
         <f>K46*A46</f>
-        <v>8.76</v>
+        <v>5.84</v>
       </c>
       <c r="N46" s="6">
         <f>L46*A46</f>
-        <v>8.76</v>
+        <v>5.84</v>
       </c>
       <c r="O46" s="11"/>
       <c r="P46" s="4" t="str">
-        <f>IF(NOT(I46=""),A46&amp;","&amp;I46,"")</f>
-        <v>3,TC4424EPA-ND</v>
+        <f t="shared" si="17"/>
+        <v>2,TC4424EPA-ND</v>
       </c>
       <c r="Q46" t="str">
         <f>A46&amp;"x "&amp;C46</f>
-        <v>3x TC4424EPA</v>
+        <v>2x TC4424EPA</v>
       </c>
       <c r="R46" t="str">
-        <f>IF(NOT(J46=""),J46&amp;"|"&amp;A46,"")</f>
-        <v>579-TC4424EPA|3</v>
+        <f t="shared" si="18"/>
+        <v>579-TC4424EPA|2</v>
       </c>
       <c r="S46" t="str">
         <f>H46&amp;" "&amp;A46</f>
-        <v>TC4424EPA 3</v>
+        <v>TC4424EPA 2</v>
       </c>
     </row>
     <row r="47" spans="1:19" ht="16.5" thickBot="1">
       <c r="A47" s="17">
-        <f>LEN(B47)-LEN(SUBSTITUTE(B47,",",""))+1</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="B47" s="11" t="s">
@@ -4652,7 +4644,7 @@
       </c>
       <c r="O47" s="4"/>
       <c r="P47" s="4" t="str">
-        <f>IF(NOT(I47=""),A47&amp;","&amp;I47,"")</f>
+        <f t="shared" si="17"/>
         <v>1,F2720-ND</v>
       </c>
       <c r="Q47" t="str">
@@ -4660,7 +4652,7 @@
         <v>1x SP721APP</v>
       </c>
       <c r="R47" t="str">
-        <f>IF(NOT(J47=""),J47&amp;"|"&amp;A47,"")</f>
+        <f t="shared" si="18"/>
         <v>576-SP721APP|1</v>
       </c>
       <c r="S47" t="str">
@@ -4670,17 +4662,17 @@
     </row>
     <row r="48" spans="1:19" ht="16.5" thickBot="1">
       <c r="A48" s="17">
-        <f>LEN(B48)-LEN(SUBSTITUTE(B48,",",""))+1</f>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>217</v>
@@ -4690,13 +4682,13 @@
         <v>38</v>
       </c>
       <c r="H48" s="12" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="I48" s="12" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="K48" s="6">
         <v>1.41</v>
@@ -4714,7 +4706,7 @@
       </c>
       <c r="O48" s="4"/>
       <c r="P48" s="4" t="str">
-        <f>IF(NOT(I48=""),A48&amp;","&amp;I48,"")</f>
+        <f t="shared" si="17"/>
         <v>2,497-14323-1-ND</v>
       </c>
       <c r="Q48" t="str">
@@ -4722,7 +4714,7 @@
         <v>2x VNLD5090TR-E</v>
       </c>
       <c r="R48" t="str">
-        <f>IF(NOT(J48=""),J48&amp;"|"&amp;A48,"")</f>
+        <f t="shared" si="18"/>
         <v>511-VNLD5090TR-E|2</v>
       </c>
       <c r="S48" t="str">
@@ -4747,11 +4739,11 @@
       <c r="N49" s="6"/>
       <c r="O49" s="9"/>
       <c r="P49" s="4" t="str">
-        <f>IF(NOT(I49=""),A49&amp;","&amp;I49,"")</f>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="R49" t="str">
-        <f>IF(NOT(J49=""),J49&amp;"|"&amp;A49,"")</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
     </row>
@@ -4774,11 +4766,11 @@
       <c r="N50" s="6"/>
       <c r="O50" s="9"/>
       <c r="P50" s="4" t="str">
-        <f>IF(NOT(I50=""),A50&amp;","&amp;I50,"")</f>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="R50" t="str">
-        <f>IF(NOT(J50=""),J50&amp;"|"&amp;A50,"")</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
     </row>
@@ -5103,11 +5095,11 @@
       <c r="L58" s="1"/>
       <c r="M58" s="10">
         <f>SUM(M3:M53)</f>
-        <v>108.52</v>
+        <v>95.07</v>
       </c>
       <c r="N58" s="10">
         <f>SUM(N3:N53)</f>
-        <v>125.712</v>
+        <v>114.45200000000001</v>
       </c>
       <c r="O58" s="9" t="s">
         <v>65</v>

</xml_diff>